<commit_message>
Fix excel upload error
</commit_message>
<xml_diff>
--- a/G3/wwwroot/Template/Template.xlsx
+++ b/G3/wwwroot/Template/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dotnet_project\g3\G3\wwwroot\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E205CAF7-2E49-4B3A-B2B5-88E20EA0616F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8209BE24-80F6-4BEA-9074-3E4A80F5840A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="3105" windowWidth="23760" windowHeight="11385" xr2:uid="{C730A044-E656-49C8-B381-0FFC7C906719}"/>
+    <workbookView xWindow="2040" yWindow="2940" windowWidth="23760" windowHeight="11385" xr2:uid="{C730A044-E656-49C8-B381-0FFC7C906719}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Email</t>
   </si>
@@ -45,18 +45,10 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>Joever@gmail.com</t>
-  </si>
-  <si>
-    <t>joe biden</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>*DO NOT DELETE TITLE ROW
 - Gender is either Male or Femail
-- Email is either @gmail.com or @fpt.edu.vn</t>
+- Email is either @gmail.com or @fpt.edu.vn
+- DO NOT make gmail into a url/link, it will bug</t>
   </si>
 </sst>
 </file>
@@ -425,7 +417,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,20 +440,12 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="E3" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -471,9 +455,6 @@
       <c r="A5" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{209BB068-80F9-4B65-A685-174AA4CF8AB2}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix inter 1 add paging, search, fix layout fix inter 2 excel, add student, fix layout
</commit_message>
<xml_diff>
--- a/G3/wwwroot/Template/Template.xlsx
+++ b/G3/wwwroot/Template/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dotnet_project\g3\G3\wwwroot\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8209BE24-80F6-4BEA-9074-3E4A80F5840A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD736EC-30B1-4E94-B642-2C0B5C0DE270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="2940" windowWidth="23760" windowHeight="11385" xr2:uid="{C730A044-E656-49C8-B381-0FFC7C906719}"/>
   </bookViews>
@@ -42,11 +42,11 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Gender</t>
+    <t>Status</t>
   </si>
   <si>
     <t>*DO NOT DELETE TITLE ROW
-- Gender is either Male or Femail
+- Status is either 1 or 0 (1 is true, 0 is false)
 - Email is either @gmail.com or @fpt.edu.vn
 - DO NOT make gmail into a url/link, it will bug</t>
   </si>
@@ -417,7 +417,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +442,7 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="E3" s="2" t="s">
         <v>3</v>

</xml_diff>